<commit_message>
more poly fits for thing
</commit_message>
<xml_diff>
--- a/test/writer_output/Molar Volume Analysis.xlsx
+++ b/test/writer_output/Molar Volume Analysis.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Membrane Libraries\SorptionModels.jl\test\writer_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA0CF7F-22FA-4EAA-9E42-6B327DA2D56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Partial Molar Volume Analysis" sheetId="2" r:id="rId2"/>
-    <sheet name="Also with uncertainty!" sheetId="3" r:id="rId3"/>
+    <sheet name="Partial Molar Volume Analysis" r:id="rId4" sheetId="2"/>
+    <sheet name="Also with uncertainty!" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Step</t>
   </si>
@@ -407,26 +407,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A55580D-D8EE-41A6-AA8F-7F3E379B46E2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD74C6A-B4A0-4F73-B900-482C8AFAD893}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,12 +455,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -472,19 +472,19 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>1.0865252000850483E-2</v>
+        <v>0.01053987096240326</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2">
-        <v>52.80069935559932</v>
+        <v>51.21948003498717</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -501,24 +501,24 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <v>1.1026465701141295E-2</v>
+        <v>0.011113095737457345</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3">
-        <v>53.584132277393735</v>
+        <v>54.00511896986348</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.2247842855431781</v>
+        <v>4.224784285543178</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -530,24 +530,24 @@
         <v>9</v>
       </c>
       <c r="F4">
-        <v>1.1434777612707274E-2</v>
+        <v>0.011370306108005027</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4">
-        <v>55.568361863989395</v>
+        <v>55.25505661009192</v>
       </c>
       <c r="I4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.9819954485567139</v>
+        <v>5.981995448556714</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -559,24 +559,24 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>1.1406650821340847E-2</v>
+        <v>0.011461576737019237</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
       <c r="H5">
-        <v>55.431677113864858</v>
+        <v>55.698594692982084</v>
       </c>
       <c r="I5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.9448377051143853</v>
+        <v>7.944837705114385</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -588,24 +588,24 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>1.1592806793243118E-2</v>
+        <v>0.011607112618723691</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
       </c>
       <c r="H6">
-        <v>56.336319316815313</v>
+        <v>56.405839801952176</v>
       </c>
       <c r="I6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>9.8889862258953158</v>
+        <v>9.888986225895316</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -617,19 +617,19 @@
         <v>9</v>
       </c>
       <c r="F7">
-        <v>1.2109487935165813E-2</v>
+        <v>0.011959847739864717</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
       </c>
       <c r="H7">
-        <v>58.847179224641891</v>
+        <v>58.11998882326069</v>
       </c>
       <c r="I7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -646,13 +646,13 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <v>1.2120110293003685E-2</v>
+        <v>0.01264874296840362</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8">
-        <v>58.898799557295121</v>
+        <v>61.467739050014956</v>
       </c>
       <c r="I8" t="s">
         <v>9</v>
@@ -664,25 +664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5718D0B5-B8A2-4708-B997-64DF0AD70B35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="A1:J8"/>
-    </sheetView>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,36 +700,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="C2">
-        <v>4.6734339441849319E-3</v>
+        <v>0.004673433944184932</v>
       </c>
       <c r="D2">
         <v>0.21681059625562235</v>
       </c>
       <c r="E2">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F2">
-        <v>1.0865252000850483E-2</v>
+        <v>0.010539870962403301</v>
       </c>
       <c r="G2">
-        <v>6.4416278126297282E-4</v>
+        <v>0.0013482065001652753</v>
       </c>
       <c r="H2">
-        <v>52.80069935559932</v>
+        <v>51.21948003498738</v>
       </c>
       <c r="I2">
-        <v>3.1822690079856573</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6.5752203803287195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -748,120 +737,120 @@
         <v>2.0282703317762607</v>
       </c>
       <c r="C3">
-        <v>2.2478706378621635E-2</v>
+        <v>0.022478706378621635</v>
       </c>
       <c r="D3">
         <v>0.21681059625562235</v>
       </c>
       <c r="E3">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F3">
-        <v>1.1026465701141295E-2</v>
+        <v>0.011113095737457345</v>
       </c>
       <c r="G3">
-        <v>3.0926910483063732E-4</v>
+        <v>0.00030566353984542554</v>
       </c>
       <c r="H3">
-        <v>53.584132277393735</v>
+        <v>54.00511896986348</v>
       </c>
       <c r="I3">
-        <v>1.6112716139585448</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.596608553343804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.2247842855431781</v>
+        <v>4.224784285543178</v>
       </c>
       <c r="C4">
-        <v>4.6036726925799798E-2</v>
+        <v>0.0460367269257998</v>
       </c>
       <c r="D4">
         <v>0.21681059625562235</v>
       </c>
       <c r="E4">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F4">
-        <v>1.1434777612707274E-2</v>
+        <v>0.011370306108005017</v>
       </c>
       <c r="G4">
-        <v>3.3051072387096795E-4</v>
+        <v>0.00036816970517249717</v>
       </c>
       <c r="H4">
-        <v>55.568361863989395</v>
+        <v>55.25505661009188</v>
       </c>
       <c r="I4">
-        <v>1.7153961916228193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.8867614750867665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.9819954485567139</v>
+        <v>5.981995448556714</v>
       </c>
       <c r="C5">
-        <v>6.501618328409213E-2</v>
+        <v>0.06501618328409213</v>
       </c>
       <c r="D5">
         <v>0.21681059625562235</v>
       </c>
       <c r="E5">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F5">
-        <v>1.1406650821340847E-2</v>
+        <v>0.011461576737019233</v>
       </c>
       <c r="G5">
-        <v>3.5126856120105032E-4</v>
+        <v>0.0002461288425864187</v>
       </c>
       <c r="H5">
-        <v>55.431677113864858</v>
+        <v>55.69859469298207</v>
       </c>
       <c r="I5">
-        <v>1.8097005003940558</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.3398502660856424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.9448377051143853</v>
+        <v>7.944837705114385</v>
       </c>
       <c r="C6">
-        <v>8.6252953131432913E-2</v>
+        <v>0.08625295313143291</v>
       </c>
       <c r="D6">
         <v>0.21681059625562235</v>
       </c>
       <c r="E6">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F6">
-        <v>1.1592806793243118E-2</v>
+        <v>0.011607112618723695</v>
       </c>
       <c r="G6">
-        <v>3.3447976873186695E-4</v>
+        <v>0.0003781153869899814</v>
       </c>
       <c r="H6">
-        <v>56.336319316815313</v>
+        <v>56.4058398019522</v>
       </c>
       <c r="I6">
-        <v>1.7363795277157446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.9365567949520686</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>9.8889862258953158</v>
+        <v>9.888986225895316</v>
       </c>
       <c r="C7">
         <v>0.10730367015276393</v>
@@ -870,22 +859,22 @@
         <v>0.21681059625562235</v>
       </c>
       <c r="E7">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F7">
-        <v>1.2109487935165813E-2</v>
+        <v>0.011959847739864716</v>
       </c>
       <c r="G7">
-        <v>3.431519993561229E-4</v>
+        <v>0.0003080436305770664</v>
       </c>
       <c r="H7">
-        <v>58.847179224641891</v>
+        <v>58.119988823260684</v>
       </c>
       <c r="I7">
-        <v>1.78543555414885</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.6241532556642557</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -899,19 +888,19 @@
         <v>0.21681059625562235</v>
       </c>
       <c r="E8">
-        <v>2.3503417324359246E-3</v>
+        <v>0.0023503417324359246</v>
       </c>
       <c r="F8">
-        <v>1.2120110293003685E-2</v>
+        <v>0.012648742968403584</v>
       </c>
       <c r="G8">
-        <v>7.0092681644138611E-4</v>
+        <v>0.0013179241631915053</v>
       </c>
       <c r="H8">
-        <v>58.898799557295121</v>
+        <v>61.467739050014785</v>
       </c>
       <c r="I8">
-        <v>3.4655449274318837</v>
+        <v>6.439145069972003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rewrote partial immobilization writer
</commit_message>
<xml_diff>
--- a/test/writer_output/Molar Volume Analysis.xlsx
+++ b/test/writer_output/Molar Volume Analysis.xlsx
@@ -582,7 +582,7 @@
         <v>27</v>
       </c>
       <c r="F2">
-        <v>0.17817941175298221</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
@@ -606,7 +606,7 @@
         <v>27</v>
       </c>
       <c r="N2">
-        <v>43.114462213408345</v>
+        <v>52.46213447313791</v>
       </c>
       <c r="O2" t="s">
         <v>27</v>
@@ -630,7 +630,7 @@
         <v>27</v>
       </c>
       <c r="V2">
-        <v>0.17817941175298221</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W2" t="s">
         <v>27</v>
@@ -642,7 +642,7 @@
         <v>27</v>
       </c>
       <c r="Z2">
-        <v>43.114462213408345</v>
+        <v>52.46213447313791</v>
       </c>
       <c r="AA2" t="s">
         <v>27</v>
@@ -659,13 +659,13 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <v>2.449497352479485</v>
+        <v>2.0282703317762607</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3">
-        <v>0.18083674421695575</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -689,7 +689,7 @@
         <v>27</v>
       </c>
       <c r="N3">
-        <v>43.76807609938999</v>
+        <v>52.47485911759988</v>
       </c>
       <c r="O3" t="s">
         <v>27</v>
@@ -707,13 +707,13 @@
         <v>27</v>
       </c>
       <c r="T3">
-        <v>0.49240731844863606</v>
+        <v>0.4052995299870725</v>
       </c>
       <c r="U3" t="s">
         <v>27</v>
       </c>
       <c r="V3">
-        <v>0.17873180797546914</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W3" t="s">
         <v>27</v>
@@ -725,7 +725,7 @@
         <v>27</v>
       </c>
       <c r="Z3">
-        <v>43.44015307148589</v>
+        <v>52.69507199388379</v>
       </c>
       <c r="AA3" t="s">
         <v>27</v>
@@ -742,13 +742,13 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <v>5.063901037152608</v>
+        <v>4.224784285543178</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4">
-        <v>0.1834344556960193</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -772,7 +772,7 @@
         <v>27</v>
       </c>
       <c r="N4">
-        <v>44.40872802313298</v>
+        <v>52.48895451574734</v>
       </c>
       <c r="O4" t="s">
         <v>27</v>
@@ -790,13 +790,13 @@
         <v>27</v>
       </c>
       <c r="T4">
-        <v>0.9833101884528241</v>
+        <v>0.810599059974145</v>
       </c>
       <c r="U4" t="s">
         <v>27</v>
       </c>
       <c r="V4">
-        <v>0.17927325903075117</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W4" t="s">
         <v>27</v>
@@ -808,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="Z4">
-        <v>43.76434739316399</v>
+        <v>52.92799553235364</v>
       </c>
       <c r="AA4" t="s">
         <v>27</v>
@@ -825,13 +825,13 @@
         <v>27</v>
       </c>
       <c r="D5">
-        <v>7.13005651985377</v>
+        <v>5.981995448556714</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
       </c>
       <c r="F5">
-        <v>0.18532627603702329</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -855,7 +855,7 @@
         <v>27</v>
       </c>
       <c r="N5">
-        <v>44.87657045946695</v>
+        <v>52.500466783677986</v>
       </c>
       <c r="O5" t="s">
         <v>27</v>
@@ -873,13 +873,13 @@
         <v>27</v>
       </c>
       <c r="T5">
-        <v>1.4727472515695061</v>
+        <v>1.2158985899612178</v>
       </c>
       <c r="U5" t="s">
         <v>27</v>
       </c>
       <c r="V5">
-        <v>0.17980402772424994</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W5" t="s">
         <v>27</v>
@@ -891,7 +891,7 @@
         <v>27</v>
       </c>
       <c r="Z5">
-        <v>44.08707423745635</v>
+        <v>53.16090508966752</v>
       </c>
       <c r="AA5" t="s">
         <v>27</v>
@@ -908,13 +908,13 @@
         <v>27</v>
       </c>
       <c r="D6">
-        <v>9.414252357674307</v>
+        <v>7.944837705114385</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>
       </c>
       <c r="F6">
-        <v>0.18726488102959535</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
@@ -938,7 +938,7 @@
         <v>27</v>
       </c>
       <c r="N6">
-        <v>45.35732286024531</v>
+        <v>52.513574140654804</v>
       </c>
       <c r="O6" t="s">
         <v>27</v>
@@ -956,13 +956,13 @@
         <v>27</v>
       </c>
       <c r="T6">
-        <v>1.9607558372517362</v>
+        <v>1.62119811994829</v>
       </c>
       <c r="U6" t="s">
         <v>27</v>
       </c>
       <c r="V6">
-        <v>0.18032436995235632</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W6" t="s">
         <v>27</v>
@@ -974,7 +974,7 @@
         <v>27</v>
       </c>
       <c r="Z6">
-        <v>44.40836209534838</v>
+        <v>53.393800666942234</v>
       </c>
       <c r="AA6" t="s">
         <v>27</v>
@@ -991,13 +991,13 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>11.65449221043736</v>
+        <v>9.888986225895316</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7">
-        <v>0.18902199523337998</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
@@ -1021,7 +1021,7 @@
         <v>27</v>
       </c>
       <c r="N7">
-        <v>45.79445583993324</v>
+        <v>52.52681447785474</v>
       </c>
       <c r="O7" t="s">
         <v>27</v>
@@ -1039,13 +1039,13 @@
         <v>27</v>
       </c>
       <c r="T7">
-        <v>2.4473720180717717</v>
+        <v>2.0264976499353624</v>
       </c>
       <c r="U7" t="s">
         <v>27</v>
       </c>
       <c r="V7">
-        <v>0.18083453487483386</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W7" t="s">
         <v>27</v>
@@ -1057,7 +1057,7 @@
         <v>27</v>
       </c>
       <c r="Z7">
-        <v>44.72823889517048</v>
+        <v>53.62668226529891</v>
       </c>
       <c r="AA7" t="s">
         <v>27</v>
@@ -1074,13 +1074,13 @@
         <v>27</v>
       </c>
       <c r="D8">
-        <v>13.784494468595295</v>
+        <v>11.753686369625104</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
       </c>
       <c r="F8">
-        <v>0.19057053593990395</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
@@ -1104,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="N8">
-        <v>46.18099572351015</v>
+        <v>52.539754737584474</v>
       </c>
       <c r="O8" t="s">
         <v>27</v>
@@ -1122,13 +1122,13 @@
         <v>27</v>
       </c>
       <c r="T8">
-        <v>2.932630662178406</v>
+        <v>2.4317971799224356</v>
       </c>
       <c r="U8" t="s">
         <v>27</v>
       </c>
       <c r="V8">
-        <v>0.18133476508491816</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W8" t="s">
         <v>27</v>
@@ -1140,7 +1140,7 @@
         <v>27</v>
       </c>
       <c r="Z8">
-        <v>45.046732008504215</v>
+        <v>53.859549885855444</v>
       </c>
       <c r="AA8" t="s">
         <v>27</v>
@@ -1160,13 +1160,13 @@
         <v>27</v>
       </c>
       <c r="T9">
-        <v>3.416565483148806</v>
+        <v>2.837096709909508</v>
       </c>
       <c r="U9" t="s">
         <v>27</v>
       </c>
       <c r="V9">
-        <v>0.18182529677691842</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W9" t="s">
         <v>27</v>
@@ -1178,7 +1178,7 @@
         <v>27</v>
       </c>
       <c r="Z9">
-        <v>45.3638682565769</v>
+        <v>54.09240352972972</v>
       </c>
       <c r="AA9" t="s">
         <v>27</v>
@@ -1198,13 +1198,13 @@
         <v>27</v>
       </c>
       <c r="T10">
-        <v>3.899209087384611</v>
+        <v>3.24239623989658</v>
       </c>
       <c r="U10" t="s">
         <v>27</v>
       </c>
       <c r="V10">
-        <v>0.18230635991115746</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W10" t="s">
         <v>27</v>
@@ -1216,7 +1216,7 @@
         <v>27</v>
       </c>
       <c r="Z10">
-        <v>45.67967391707289</v>
+        <v>54.32524319803964</v>
       </c>
       <c r="AA10" t="s">
         <v>27</v>
@@ -1236,13 +1236,13 @@
         <v>27</v>
       </c>
       <c r="T11">
-        <v>4.380593019192256</v>
+        <v>3.6476957698836525</v>
       </c>
       <c r="U11" t="s">
         <v>27</v>
       </c>
       <c r="V11">
-        <v>0.1827781783761104</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W11" t="s">
         <v>27</v>
@@ -1254,7 +1254,7 @@
         <v>27</v>
       </c>
       <c r="Z11">
-        <v>45.99417473131174</v>
+        <v>54.55806889190634</v>
       </c>
       <c r="AA11" t="s">
         <v>27</v>
@@ -1274,13 +1274,13 @@
         <v>27</v>
       </c>
       <c r="T12">
-        <v>4.860747803678475</v>
+        <v>4.052995299870725</v>
       </c>
       <c r="U12" t="s">
         <v>27</v>
       </c>
       <c r="V12">
-        <v>0.183240970147628</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W12" t="s">
         <v>27</v>
@@ -1292,7 +1292,7 @@
         <v>27</v>
       </c>
       <c r="Z12">
-        <v>46.30739591173015</v>
+        <v>54.790880612445534</v>
       </c>
       <c r="AA12" t="s">
         <v>27</v>
@@ -1312,13 +1312,13 @@
         <v>27</v>
       </c>
       <c r="T13">
-        <v>5.339702987583527</v>
+        <v>4.458294829857798</v>
       </c>
       <c r="U13" t="s">
         <v>27</v>
       </c>
       <c r="V13">
-        <v>0.18369494744514867</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W13" t="s">
         <v>27</v>
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="Z13">
-        <v>46.619362149646946</v>
+        <v>55.02367836077728</v>
       </c>
       <c r="AA13" t="s">
         <v>27</v>
@@ -1350,13 +1350,13 @@
         <v>27</v>
       </c>
       <c r="T14">
-        <v>5.817487178166894</v>
+        <v>4.863594359844871</v>
       </c>
       <c r="U14" t="s">
         <v>27</v>
       </c>
       <c r="V14">
-        <v>0.18414031688482524</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W14" t="s">
         <v>27</v>
@@ -1368,7 +1368,7 @@
         <v>27</v>
       </c>
       <c r="Z14">
-        <v>46.9300976232392</v>
+        <v>55.2564621380184</v>
       </c>
       <c r="AA14" t="s">
         <v>27</v>
@@ -1388,13 +1388,13 @@
         <v>27</v>
       </c>
       <c r="T15">
-        <v>6.294128080252962</v>
+        <v>5.2688938898319435</v>
       </c>
       <c r="U15" t="s">
         <v>27</v>
       </c>
       <c r="V15">
-        <v>0.1845772796295066</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W15" t="s">
         <v>27</v>
@@ -1406,7 +1406,7 @@
         <v>27</v>
       </c>
       <c r="Z15">
-        <v>47.23962600571443</v>
+        <v>55.4892319452857</v>
       </c>
       <c r="AA15" t="s">
         <v>27</v>
@@ -1426,13 +1426,13 @@
         <v>27</v>
       </c>
       <c r="T16">
-        <v>6.769652531537481</v>
+        <v>5.674193419819016</v>
       </c>
       <c r="U16" t="s">
         <v>27</v>
       </c>
       <c r="V16">
-        <v>0.18500603153553227</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W16" t="s">
         <v>27</v>
@@ -1444,7 +1444,7 @@
         <v>27</v>
       </c>
       <c r="Z16">
-        <v>47.547970473636255</v>
+        <v>55.7219877837003</v>
       </c>
       <c r="AA16" t="s">
         <v>27</v>
@@ -1464,13 +1464,13 @@
         <v>27</v>
       </c>
       <c r="T17">
-        <v>7.244086536249314</v>
+        <v>6.079492949806087</v>
       </c>
       <c r="U17" t="s">
         <v>27</v>
       </c>
       <c r="V17">
-        <v>0.1854267632963093</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W17" t="s">
         <v>27</v>
@@ -1482,7 +1482,7 @@
         <v>27</v>
       </c>
       <c r="Z17">
-        <v>47.85515371535657</v>
+        <v>55.9547296543758</v>
       </c>
       <c r="AA17" t="s">
         <v>27</v>
@@ -1502,13 +1502,13 @@
         <v>27</v>
       </c>
       <c r="T18">
-        <v>7.717455297256173</v>
+        <v>6.48479247979316</v>
       </c>
       <c r="U18" t="s">
         <v>27</v>
       </c>
       <c r="V18">
-        <v>0.1858396605826547</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W18" t="s">
         <v>27</v>
@@ -1520,7 +1520,7 @@
         <v>27</v>
       </c>
       <c r="Z18">
-        <v>48.161197939561404</v>
+        <v>56.18745755843222</v>
       </c>
       <c r="AA18" t="s">
         <v>27</v>
@@ -1540,13 +1540,13 @@
         <v>27</v>
       </c>
       <c r="T19">
-        <v>8.189783246697617</v>
+        <v>6.890092009780233</v>
       </c>
       <c r="U19" t="s">
         <v>27</v>
       </c>
       <c r="V19">
-        <v>0.18624490417989684</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W19" t="s">
         <v>27</v>
@@ -1558,7 +1558,7 @@
         <v>27</v>
       </c>
       <c r="Z19">
-        <v>48.46612488386201</v>
+        <v>56.4201714969864</v>
       </c>
       <c r="AA19" t="s">
         <v>27</v>
@@ -1578,13 +1578,13 @@
         <v>27</v>
       </c>
       <c r="T20">
-        <v>8.661094075223545</v>
+        <v>7.295391539767305</v>
       </c>
       <c r="U20" t="s">
         <v>27</v>
       </c>
       <c r="V20">
-        <v>0.18664267012173855</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W20" t="s">
         <v>27</v>
@@ -1596,7 +1596,7 @@
         <v>27</v>
       </c>
       <c r="Z20">
-        <v>48.76995582343942</v>
+        <v>56.6528714711562</v>
       </c>
       <c r="AA20" t="s">
         <v>27</v>
@@ -1616,13 +1616,13 @@
         <v>27</v>
       </c>
       <c r="T21">
-        <v>9.131410759911658</v>
+        <v>7.700691069754377</v>
       </c>
       <c r="U21" t="s">
         <v>27</v>
       </c>
       <c r="V21">
-        <v>0.18703312982089454</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W21" t="s">
         <v>27</v>
@@ -1634,7 +1634,7 @@
         <v>27</v>
       </c>
       <c r="Z21">
-        <v>49.07271157970491</v>
+        <v>56.88555748205955</v>
       </c>
       <c r="AA21" t="s">
         <v>27</v>
@@ -1654,13 +1654,13 @@
         <v>27</v>
       </c>
       <c r="T22">
-        <v>9.600755590933032</v>
+        <v>8.10599059974145</v>
       </c>
       <c r="U22" t="s">
         <v>27</v>
       </c>
       <c r="V22">
-        <v>0.18741645019652103</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W22" t="s">
         <v>27</v>
@@ -1672,7 +1672,7 @@
         <v>27</v>
       </c>
       <c r="Z22">
-        <v>49.37441252896012</v>
+        <v>57.118229530812165</v>
       </c>
       <c r="AA22" t="s">
         <v>27</v>
@@ -1692,13 +1692,13 @@
         <v>27</v>
       </c>
       <c r="T23">
-        <v>10.069150197030792</v>
+        <v>8.511290129728524</v>
       </c>
       <c r="U23" t="s">
         <v>27</v>
       </c>
       <c r="V23">
-        <v>0.18779279379846484</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W23" t="s">
         <v>27</v>
@@ -1710,7 +1710,7 @@
         <v>27</v>
       </c>
       <c r="Z23">
-        <v>49.67507861104553</v>
+        <v>57.350887618530855</v>
       </c>
       <c r="AA23" t="s">
         <v>27</v>
@@ -1730,13 +1730,13 @@
         <v>27</v>
       </c>
       <c r="T24">
-        <v>10.53661556987307</v>
+        <v>8.916589659715596</v>
       </c>
       <c r="U24" t="s">
         <v>27</v>
       </c>
       <c r="V24">
-        <v>0.18816231892836266</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W24" t="s">
         <v>27</v>
@@ -1748,7 +1748,7 @@
         <v>27</v>
       </c>
       <c r="Z24">
-        <v>49.97472933795472</v>
+        <v>57.58353174633459</v>
       </c>
       <c r="AA24" t="s">
         <v>27</v>
@@ -1768,13 +1768,13 @@
         <v>27</v>
       </c>
       <c r="T25">
-        <v>11.003172087337875</v>
+        <v>9.321889189702668</v>
       </c>
       <c r="U25" t="s">
         <v>27</v>
       </c>
       <c r="V25">
-        <v>0.18852517975762803</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W25" t="s">
         <v>27</v>
@@ -1786,7 +1786,7 @@
         <v>27</v>
       </c>
       <c r="Z25">
-        <v>50.27338380239604</v>
+        <v>57.816161915338036</v>
       </c>
       <c r="AA25" t="s">
         <v>27</v>
@@ -1806,13 +1806,13 @@
         <v>27</v>
       </c>
       <c r="T26">
-        <v>11.468839535784081</v>
+        <v>9.727188719689742</v>
       </c>
       <c r="U26" t="s">
         <v>27</v>
       </c>
       <c r="V26">
-        <v>0.18888152644236633</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W26" t="s">
         <v>27</v>
@@ -1824,7 +1824,7 @@
         <v>27</v>
       </c>
       <c r="Z26">
-        <v>50.571060686307604</v>
+        <v>58.04877812665908</v>
       </c>
       <c r="AA26" t="s">
         <v>27</v>
@@ -1844,13 +1844,13 @@
         <v>27</v>
       </c>
       <c r="T27">
-        <v>11.933637131359704</v>
+        <v>10.132488249676813</v>
       </c>
       <c r="U27" t="s">
         <v>27</v>
       </c>
       <c r="V27">
-        <v>0.18923150523526344</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W27" t="s">
         <v>27</v>
@@ -1862,7 +1862,7 @@
         <v>27</v>
       </c>
       <c r="Z27">
-        <v>50.86777826929122</v>
+        <v>58.28138038141345</v>
       </c>
       <c r="AA27" t="s">
         <v>27</v>
@@ -1882,13 +1882,13 @@
         <v>27</v>
       </c>
       <c r="T28">
-        <v>12.397583540395692</v>
+        <v>10.537787779663887</v>
       </c>
       <c r="U28" t="s">
         <v>27</v>
       </c>
       <c r="V28">
-        <v>0.18957525859449623</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W28" t="s">
         <v>27</v>
@@ -1900,7 +1900,7 @@
         <v>27</v>
       </c>
       <c r="Z28">
-        <v>51.16355443697323</v>
+        <v>58.51396868071689</v>
       </c>
       <c r="AA28" t="s">
         <v>27</v>
@@ -1920,13 +1920,13 @@
         <v>27</v>
       </c>
       <c r="T29">
-        <v>12.860696898930597</v>
+        <v>10.943087309650958</v>
       </c>
       <c r="U29" t="s">
         <v>27</v>
       </c>
       <c r="V29">
-        <v>0.18991292528971457</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W29" t="s">
         <v>27</v>
@@ -1938,7 +1938,7 @@
         <v>27</v>
       </c>
       <c r="Z29">
-        <v>51.458406689278426</v>
+        <v>58.74654302568944</v>
       </c>
       <c r="AA29" t="s">
         <v>27</v>
@@ -1958,13 +1958,13 @@
         <v>27</v>
       </c>
       <c r="T30">
-        <v>13.322994831409183</v>
+        <v>11.348386839638032</v>
       </c>
       <c r="U30" t="s">
         <v>27</v>
       </c>
       <c r="V30">
-        <v>0.19024464050514997</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W30" t="s">
         <v>27</v>
@@ -1976,7 +1976,7 @@
         <v>27</v>
       </c>
       <c r="Z30">
-        <v>51.752352148594085</v>
+        <v>58.97910341744361</v>
       </c>
       <c r="AA30" t="s">
         <v>27</v>
@@ -1996,13 +1996,13 @@
         <v>27</v>
       </c>
       <c r="T31">
-        <v>13.784494468595295</v>
+        <v>11.753686369625104</v>
       </c>
       <c r="U31" t="s">
         <v>27</v>
       </c>
       <c r="V31">
-        <v>0.19057053593990395</v>
+        <v>0.21681059625562235</v>
       </c>
       <c r="W31" t="s">
         <v>27</v>
@@ -2014,7 +2014,7 @@
         <v>27</v>
       </c>
       <c r="Z31">
-        <v>52.04540756785243</v>
+        <v>59.21164985709727</v>
       </c>
       <c r="AA31" t="s">
         <v>27</v>

</xml_diff>